<commit_message>
Release (Android) v1.1 (APK Generado)
Ahora se puede seleccionar el tipo de comision seleccionando previamente el pais de origen de la cuenta y el tipo de transaccion que se realizara.
</commit_message>
<xml_diff>
--- a/Research/Tabla de comisiones.xlsx
+++ b/Research/Tabla de comisiones.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Freddy\Development\GitHub\calculadora-paypal\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF884A6-D5D1-4E3D-B0A4-53C19F60FE89}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196D3B62-924F-4801-88A1-B6CCEFEAD5ED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{4E86ACBF-E339-409F-9C61-B3854862241B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{4E86ACBF-E339-409F-9C61-B3854862241B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Investigacion" sheetId="1" r:id="rId1"/>
+    <sheet name="Estados Unidos (USD)" sheetId="2" r:id="rId2"/>
+    <sheet name="Otros Paises (USD)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
   <si>
     <t>Divisa</t>
   </si>
@@ -124,13 +126,58 @@
   </si>
   <si>
     <t>Domestical Transfer</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t>Opciones</t>
+  </si>
+  <si>
+    <t>Transferencia Internacional (Otros paises): Financiado por TDD/TDC/CreditoPayPal</t>
+  </si>
+  <si>
+    <t>Transferencia Internacional (Canada o Europa): Financiado por el balance PayPal o de cuenta bancaria vinculada a PayPal</t>
+  </si>
+  <si>
+    <t>Transferencia Internacional (Canada o Europa): Financiado por tarjeta de debito/credito o credito PayPal</t>
+  </si>
+  <si>
+    <t>Transferencia Internacional (Otros paises): Financiado por el balance PayPal o de cuenta bancaria vinculada a PayPal</t>
+  </si>
+  <si>
+    <t>Transferencia Domestica: Financiado por el balance PayPal o de cuenta bancaria vinculada a PayPal</t>
+  </si>
+  <si>
+    <t>Transferencia Domestica: Financiado por tarjeta de debito/credito o credito PayPal</t>
+  </si>
+  <si>
+    <t>Ventas: En el interior del pais</t>
+  </si>
+  <si>
+    <t>Venta: En el exterior del pais</t>
+  </si>
+  <si>
+    <t>Estados Unidos (USD)</t>
+  </si>
+  <si>
+    <t>Pais (Divisa)</t>
+  </si>
+  <si>
+    <t>Micropagos</t>
+  </si>
+  <si>
+    <t>Obras de caridad</t>
+  </si>
+  <si>
+    <t>2.2% + $0.30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +193,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -163,11 +224,228 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -188,11 +466,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453B1BF2-953B-4211-9087-9DC9F7F7485D}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:H9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,16 +907,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -583,12 +933,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="7" t="s">
         <v>9</v>
       </c>
@@ -603,12 +953,12 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -625,12 +975,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
@@ -645,8 +995,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
@@ -656,15 +1006,15 @@
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
@@ -674,15 +1024,15 @@
       <c r="E8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
@@ -692,15 +1042,15 @@
       <c r="E9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
@@ -710,15 +1060,15 @@
       <c r="E10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
@@ -728,15 +1078,15 @@
       <c r="E11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
@@ -746,11 +1096,11 @@
       <c r="E12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -779,4 +1129,244 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC8D26F-0EB8-42D8-810B-61BC64D9973B}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A52AE2-5898-456F-B26F-C2B435CB8DF6}">
+  <dimension ref="B2:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>